<commit_message>
no new feature added , existing files have been modified.
</commit_message>
<xml_diff>
--- a/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
+++ b/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
@@ -351,12 +351,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -376,10 +377,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>37.422366400000001</v>
+        <v>37.422365800000001</v>
       </c>
       <c r="C2">
-        <v>-122.084406</v>
+        <v>-122.0843845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On failing the jira ticket created is updated in the feature file
</commit_message>
<xml_diff>
--- a/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
+++ b/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,10 +377,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>37.422365800000001</v>
+        <v>37.4224161</v>
       </c>
       <c r="C2">
-        <v>-122.0843845</v>
+        <v>-122.0842327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
relative path to feature file
</commit_message>
<xml_diff>
--- a/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
+++ b/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,10 +377,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>37.4224161</v>
+        <v>37.422341099999997</v>
       </c>
       <c r="C2">
-        <v>-122.0842327</v>
+        <v>-122.0842653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated jira time stamp code
</commit_message>
<xml_diff>
--- a/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
+++ b/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,7 +377,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>37.422341099999997</v>
+        <v>37.422349400000002</v>
       </c>
       <c r="C2">
         <v>-122.0842653</v>

</xml_diff>

<commit_message>
newfeaturecreate - changed string variable from line2 to line
</commit_message>
<xml_diff>
--- a/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
+++ b/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,10 +377,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>37.422349400000002</v>
+        <v>37.422389500000001</v>
       </c>
       <c r="C2">
-        <v>-122.0842653</v>
+        <v>-122.08431229999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
google api data resources updated to new longitude and latitude
</commit_message>
<xml_diff>
--- a/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
+++ b/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,10 +377,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>37.422389500000001</v>
+        <v>37.421654799999999</v>
       </c>
       <c r="C2">
-        <v>-122.08431229999999</v>
+        <v>-122.0856374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
google api lat and long updated in apidata
</commit_message>
<xml_diff>
--- a/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
+++ b/SpecFramework/FeatureFiles/DataResources/APIData.xlsx
@@ -351,7 +351,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,10 +377,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>37.421654799999999</v>
+        <v>37.4224082</v>
       </c>
       <c r="C2">
-        <v>-122.0856374</v>
+        <v>-122.0856086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>